<commit_message>
Add about us section
</commit_message>
<xml_diff>
--- a/input/event.xlsx
+++ b/input/event.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_7790C75EAE9ABC96DC228567D04050E0228024D1" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{957022E5-2DF0-4C52-9619-6D79B59EF968}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_7790C75EAE9ABC96DC228567D04050E0228024D1" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{1B472ABD-62F4-4567-8559-2D72D15428F4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="797" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>Name of project</t>
   </si>
@@ -211,6 +211,39 @@
   </si>
   <si>
     <t>Test in progress!</t>
+  </si>
+  <si>
+    <t>dsadsd</t>
+  </si>
+  <si>
+    <t>Planning Meetup</t>
+  </si>
+  <si>
+    <t>For Data Scientists and Stakeholders</t>
+  </si>
+  <si>
+    <t>Share, learn and have fun!</t>
+  </si>
+  <si>
+    <t>Grimross</t>
+  </si>
+  <si>
+    <t>600 Bishop Drive, Fredericton, NB E3C 0B4</t>
+  </si>
+  <si>
+    <t>This is where we'll be</t>
+  </si>
+  <si>
+    <t>Where we hang out and talk about Data Science stuff around large electrical wire spools</t>
+  </si>
+  <si>
+    <t>Meet &amp; Greet</t>
+  </si>
+  <si>
+    <t>Ideation</t>
+  </si>
+  <si>
+    <t>first event</t>
   </si>
 </sst>
 </file>
@@ -375,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +475,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2333,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B3:R20"/>
+  <dimension ref="B3:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,6 +2576,11 @@
       </c>
       <c r="R20" s="2"/>
     </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2544,8 +2591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:R32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2670,7 +2717,7 @@
         <v>-66.646791899999997</v>
       </c>
       <c r="P4" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="22">
         <v>43252</v>
@@ -2736,24 +2783,52 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+    <row r="6" spans="2:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="27">
+        <v>3</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="F6" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>63</v>
+      </c>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="23"/>
+      <c r="K6" s="22">
+        <v>43263</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="21">
+        <v>45.941000000000003</v>
+      </c>
+      <c r="O6" s="21">
+        <v>-66.67</v>
+      </c>
+      <c r="P6" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="22">
+        <v>43259</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="27"/>
@@ -3258,15 +3333,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:R25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -3439,13 +3515,27 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="B6" s="43">
+        <v>3</v>
+      </c>
+      <c r="C6" s="42">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D6" s="42">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="42">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G6" s="42">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>69</v>
+      </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -3455,7 +3545,9 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="15"/>
+      <c r="R6" s="40" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
@@ -3828,7 +3920,7 @@
   <dimension ref="B2:E40"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,10 +3974,18 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="15"/>
+      <c r="B6" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="38">
+        <v>45.941000000000003</v>
+      </c>
+      <c r="E6" s="40">
+        <v>-66.674000000000007</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>

</xml_diff>